<commit_message>
Did some patching of the SelectPeriods UserForm for error control.
</commit_message>
<xml_diff>
--- a/Sample Attendance Roster.xlsx
+++ b/Sample Attendance Roster.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15465" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -533,20 +533,24 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -650,6 +654,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -975,15 +984,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AG344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:AG345"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1024,7 +1034,7 @@
       <c r="AF1" s="4"/>
       <c r="AG1" s="4"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -1077,7 +1087,7 @@
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="6">
         <v>1</v>
@@ -1130,7 +1140,7 @@
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1181,7 +1191,7 @@
       <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>10</v>
       </c>
@@ -1222,7 +1232,7 @@
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>160</v>
       </c>
@@ -1263,7 +1273,7 @@
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>328</v>
       </c>
@@ -1304,7 +1314,7 @@
       <c r="AF7" s="4"/>
       <c r="AG7" s="4"/>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>495</v>
       </c>
@@ -1345,7 +1355,7 @@
       <c r="AF8" s="4"/>
       <c r="AG8" s="4"/>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>518</v>
       </c>
@@ -1390,7 +1400,7 @@
       <c r="AF9" s="4"/>
       <c r="AG9" s="4"/>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>538</v>
       </c>
@@ -1433,7 +1443,7 @@
       <c r="AF10" s="4"/>
       <c r="AG10" s="4"/>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>550</v>
       </c>
@@ -1474,7 +1484,7 @@
       <c r="AF11" s="4"/>
       <c r="AG11" s="4"/>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>655</v>
       </c>
@@ -1515,7 +1525,7 @@
       <c r="AF12" s="4"/>
       <c r="AG12" s="4"/>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>710</v>
       </c>
@@ -1556,7 +1566,7 @@
       <c r="AF13" s="4"/>
       <c r="AG13" s="4"/>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>774</v>
       </c>
@@ -1597,7 +1607,7 @@
       <c r="AF14" s="4"/>
       <c r="AG14" s="4"/>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>791</v>
       </c>
@@ -1642,7 +1652,7 @@
       <c r="AF15" s="4"/>
       <c r="AG15" s="4"/>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>824</v>
       </c>
@@ -1683,7 +1693,7 @@
       <c r="AF16" s="4"/>
       <c r="AG16" s="4"/>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>895</v>
       </c>
@@ -1724,7 +1734,7 @@
       <c r="AF17" s="4"/>
       <c r="AG17" s="4"/>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>906</v>
       </c>
@@ -1767,7 +1777,7 @@
       <c r="AF18" s="4"/>
       <c r="AG18" s="4"/>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>982</v>
       </c>
@@ -1808,7 +1818,7 @@
       <c r="AF19" s="4"/>
       <c r="AG19" s="4"/>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>994</v>
       </c>
@@ -1849,7 +1859,7 @@
       <c r="AF20" s="4"/>
       <c r="AG20" s="4"/>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>1060</v>
       </c>
@@ -1890,7 +1900,7 @@
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>1081</v>
       </c>
@@ -1931,7 +1941,7 @@
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>1082</v>
       </c>
@@ -1972,7 +1982,7 @@
       <c r="AF23" s="4"/>
       <c r="AG23" s="4"/>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>1100</v>
       </c>
@@ -2015,7 +2025,7 @@
       <c r="AF24" s="4"/>
       <c r="AG24" s="4"/>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>1289</v>
       </c>
@@ -2056,7 +2066,7 @@
       <c r="AF25" s="4"/>
       <c r="AG25" s="4"/>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>1190</v>
       </c>
@@ -2097,7 +2107,7 @@
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>1209</v>
       </c>
@@ -2138,7 +2148,7 @@
       <c r="AF27" s="4"/>
       <c r="AG27" s="4"/>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>1224</v>
       </c>
@@ -2179,7 +2189,7 @@
       <c r="AF28" s="4"/>
       <c r="AG28" s="4"/>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>1303</v>
       </c>
@@ -2220,7 +2230,7 @@
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>1320</v>
       </c>
@@ -2261,7 +2271,7 @@
       <c r="AF30" s="4"/>
       <c r="AG30" s="4"/>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>1360</v>
       </c>
@@ -2302,7 +2312,7 @@
       <c r="AF31" s="4"/>
       <c r="AG31" s="4"/>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>1372</v>
       </c>
@@ -2345,7 +2355,7 @@
       <c r="AF32" s="4"/>
       <c r="AG32" s="4"/>
     </row>
-    <row r="33" spans="1:33">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>1421</v>
       </c>
@@ -2386,7 +2396,7 @@
       <c r="AF33" s="4"/>
       <c r="AG33" s="4"/>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>1446</v>
       </c>
@@ -2429,7 +2439,7 @@
       <c r="AF34" s="4"/>
       <c r="AG34" s="4"/>
     </row>
-    <row r="35" spans="1:33">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>1480</v>
       </c>
@@ -2470,7 +2480,7 @@
       <c r="AF35" s="4"/>
       <c r="AG35" s="4"/>
     </row>
-    <row r="36" spans="1:33">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>1536</v>
       </c>
@@ -2511,7 +2521,7 @@
       <c r="AF36" s="4"/>
       <c r="AG36" s="4"/>
     </row>
-    <row r="37" spans="1:33">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>1552</v>
       </c>
@@ -2552,7 +2562,7 @@
       <c r="AF37" s="4"/>
       <c r="AG37" s="4"/>
     </row>
-    <row r="38" spans="1:33">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2587,7 +2597,7 @@
       <c r="AF38" s="4"/>
       <c r="AG38" s="4"/>
     </row>
-    <row r="39" spans="1:33">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2622,7 +2632,7 @@
       <c r="AF39" s="4"/>
       <c r="AG39" s="4"/>
     </row>
-    <row r="40" spans="1:33">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2657,7 +2667,7 @@
       <c r="AF40" s="4"/>
       <c r="AG40" s="4"/>
     </row>
-    <row r="41" spans="1:33">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2692,7 +2702,7 @@
       <c r="AF41" s="4"/>
       <c r="AG41" s="4"/>
     </row>
-    <row r="42" spans="1:33">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2727,7 +2737,7 @@
       <c r="AF42" s="4"/>
       <c r="AG42" s="4"/>
     </row>
-    <row r="43" spans="1:33">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2762,7 +2772,7 @@
       <c r="AF43" s="4"/>
       <c r="AG43" s="4"/>
     </row>
-    <row r="44" spans="1:33">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2797,7 +2807,7 @@
       <c r="AF44" s="4"/>
       <c r="AG44" s="4"/>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2832,7 +2842,7 @@
       <c r="AF45" s="4"/>
       <c r="AG45" s="4"/>
     </row>
-    <row r="46" spans="1:33">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -2869,7 +2879,7 @@
       <c r="AF46" s="4"/>
       <c r="AG46" s="4"/>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>56</v>
       </c>
@@ -2910,7 +2920,7 @@
       <c r="AF47" s="4"/>
       <c r="AG47" s="4"/>
     </row>
-    <row r="48" spans="1:33">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -2951,7 +2961,7 @@
       <c r="AF48" s="4"/>
       <c r="AG48" s="4"/>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="2" t="s">
         <v>2</v>
@@ -3004,7 +3014,7 @@
       <c r="AF49" s="4"/>
       <c r="AG49" s="4"/>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="6">
         <v>2</v>
@@ -3057,7 +3067,7 @@
       <c r="AF50" s="4"/>
       <c r="AG50" s="4"/>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -3108,7 +3118,7 @@
       <c r="AF51" s="4"/>
       <c r="AG51" s="4"/>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>25</v>
       </c>
@@ -3151,7 +3161,7 @@
       <c r="AF52" s="4"/>
       <c r="AG52" s="4"/>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>98</v>
       </c>
@@ -3192,7 +3202,7 @@
       <c r="AF53" s="4"/>
       <c r="AG53" s="4"/>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>231</v>
       </c>
@@ -3233,7 +3243,7 @@
       <c r="AF54" s="4"/>
       <c r="AG54" s="4"/>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
         <v>275</v>
       </c>
@@ -3274,7 +3284,7 @@
       <c r="AF55" s="4"/>
       <c r="AG55" s="4"/>
     </row>
-    <row r="56" spans="1:33">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>311</v>
       </c>
@@ -3315,7 +3325,7 @@
       <c r="AF56" s="4"/>
       <c r="AG56" s="4"/>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
         <v>392</v>
       </c>
@@ -3356,7 +3366,7 @@
       <c r="AF57" s="4"/>
       <c r="AG57" s="4"/>
     </row>
-    <row r="58" spans="1:33">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58" s="10">
         <v>521</v>
       </c>
@@ -3397,7 +3407,7 @@
       <c r="AF58" s="4"/>
       <c r="AG58" s="4"/>
     </row>
-    <row r="59" spans="1:33">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
         <v>588</v>
       </c>
@@ -3438,7 +3448,7 @@
       <c r="AF59" s="4"/>
       <c r="AG59" s="4"/>
     </row>
-    <row r="60" spans="1:33">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
         <v>593</v>
       </c>
@@ -3479,7 +3489,7 @@
       <c r="AF60" s="4"/>
       <c r="AG60" s="4"/>
     </row>
-    <row r="61" spans="1:33">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61" s="10">
         <v>690</v>
       </c>
@@ -3520,7 +3530,7 @@
       <c r="AF61" s="4"/>
       <c r="AG61" s="4"/>
     </row>
-    <row r="62" spans="1:33">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" s="10">
         <v>714</v>
       </c>
@@ -3561,7 +3571,7 @@
       <c r="AF62" s="4"/>
       <c r="AG62" s="4"/>
     </row>
-    <row r="63" spans="1:33">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A63" s="10">
         <v>767</v>
       </c>
@@ -3604,7 +3614,7 @@
       <c r="AF63" s="4"/>
       <c r="AG63" s="4"/>
     </row>
-    <row r="64" spans="1:33">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64" s="10">
         <v>947</v>
       </c>
@@ -3645,7 +3655,7 @@
       <c r="AF64" s="4"/>
       <c r="AG64" s="4"/>
     </row>
-    <row r="65" spans="1:33">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A65" s="10">
         <v>980</v>
       </c>
@@ -3686,7 +3696,7 @@
       <c r="AF65" s="4"/>
       <c r="AG65" s="4"/>
     </row>
-    <row r="66" spans="1:33">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66" s="10">
         <v>1041</v>
       </c>
@@ -3729,7 +3739,7 @@
       <c r="AF66" s="4"/>
       <c r="AG66" s="4"/>
     </row>
-    <row r="67" spans="1:33">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A67" s="10">
         <v>1043</v>
       </c>
@@ -3770,7 +3780,7 @@
       <c r="AF67" s="4"/>
       <c r="AG67" s="4"/>
     </row>
-    <row r="68" spans="1:33">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68" s="10">
         <v>1093</v>
       </c>
@@ -3811,7 +3821,7 @@
       <c r="AF68" s="4"/>
       <c r="AG68" s="4"/>
     </row>
-    <row r="69" spans="1:33">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A69" s="10">
         <v>1127</v>
       </c>
@@ -3852,7 +3862,7 @@
       <c r="AF69" s="4"/>
       <c r="AG69" s="4"/>
     </row>
-    <row r="70" spans="1:33">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A70" s="10">
         <v>1132</v>
       </c>
@@ -3897,7 +3907,7 @@
       <c r="AF70" s="4"/>
       <c r="AG70" s="4"/>
     </row>
-    <row r="71" spans="1:33">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71" s="10">
         <v>1140</v>
       </c>
@@ -3938,7 +3948,7 @@
       <c r="AF71" s="4"/>
       <c r="AG71" s="4"/>
     </row>
-    <row r="72" spans="1:33">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72" s="10">
         <v>1177</v>
       </c>
@@ -3979,7 +3989,7 @@
       <c r="AF72" s="4"/>
       <c r="AG72" s="4"/>
     </row>
-    <row r="73" spans="1:33">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A73" s="10">
         <v>1256</v>
       </c>
@@ -4020,7 +4030,7 @@
       <c r="AF73" s="4"/>
       <c r="AG73" s="4"/>
     </row>
-    <row r="74" spans="1:33">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A74" s="10">
         <v>1265</v>
       </c>
@@ -4061,7 +4071,7 @@
       <c r="AF74" s="4"/>
       <c r="AG74" s="4"/>
     </row>
-    <row r="75" spans="1:33">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75" s="10">
         <v>1321</v>
       </c>
@@ -4102,7 +4112,7 @@
       <c r="AF75" s="4"/>
       <c r="AG75" s="4"/>
     </row>
-    <row r="76" spans="1:33">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A76" s="10">
         <v>1377</v>
       </c>
@@ -4143,7 +4153,7 @@
       <c r="AF76" s="4"/>
       <c r="AG76" s="4"/>
     </row>
-    <row r="77" spans="1:33">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77" s="10">
         <v>1392</v>
       </c>
@@ -4184,7 +4194,7 @@
       <c r="AF77" s="4"/>
       <c r="AG77" s="4"/>
     </row>
-    <row r="78" spans="1:33">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78" s="10">
         <v>1433</v>
       </c>
@@ -4225,7 +4235,7 @@
       <c r="AF78" s="4"/>
       <c r="AG78" s="4"/>
     </row>
-    <row r="79" spans="1:33">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79" s="10">
         <v>1506</v>
       </c>
@@ -4270,7 +4280,7 @@
       <c r="AF79" s="4"/>
       <c r="AG79" s="4"/>
     </row>
-    <row r="80" spans="1:33">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A80" s="10">
         <v>1614</v>
       </c>
@@ -4311,7 +4321,7 @@
       <c r="AF80" s="4"/>
       <c r="AG80" s="4"/>
     </row>
-    <row r="81" spans="1:33">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -4346,7 +4356,7 @@
       <c r="AF81" s="4"/>
       <c r="AG81" s="4"/>
     </row>
-    <row r="82" spans="1:33">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -4381,7 +4391,7 @@
       <c r="AF82" s="4"/>
       <c r="AG82" s="4"/>
     </row>
-    <row r="83" spans="1:33">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -4416,7 +4426,7 @@
       <c r="AF83" s="4"/>
       <c r="AG83" s="4"/>
     </row>
-    <row r="84" spans="1:33">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -4451,7 +4461,7 @@
       <c r="AF84" s="4"/>
       <c r="AG84" s="4"/>
     </row>
-    <row r="85" spans="1:33">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -4486,7 +4496,7 @@
       <c r="AF85" s="4"/>
       <c r="AG85" s="4"/>
     </row>
-    <row r="86" spans="1:33">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -4521,7 +4531,7 @@
       <c r="AF86" s="4"/>
       <c r="AG86" s="4"/>
     </row>
-    <row r="87" spans="1:33">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -4556,7 +4566,7 @@
       <c r="AF87" s="4"/>
       <c r="AG87" s="4"/>
     </row>
-    <row r="88" spans="1:33">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -4591,7 +4601,7 @@
       <c r="AF88" s="4"/>
       <c r="AG88" s="4"/>
     </row>
-    <row r="89" spans="1:33">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -4626,7 +4636,7 @@
       <c r="AF89" s="4"/>
       <c r="AG89" s="4"/>
     </row>
-    <row r="90" spans="1:33">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -4661,7 +4671,7 @@
       <c r="AF90" s="4"/>
       <c r="AG90" s="4"/>
     </row>
-    <row r="91" spans="1:33">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -4696,7 +4706,7 @@
       <c r="AF91" s="4"/>
       <c r="AG91" s="4"/>
     </row>
-    <row r="92" spans="1:33">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -4731,7 +4741,7 @@
       <c r="AF92" s="4"/>
       <c r="AG92" s="4"/>
     </row>
-    <row r="93" spans="1:33">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -4766,7 +4776,7 @@
       <c r="AF93" s="4"/>
       <c r="AG93" s="4"/>
     </row>
-    <row r="94" spans="1:33">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -4803,7 +4813,7 @@
       <c r="AF94" s="4"/>
       <c r="AG94" s="4"/>
     </row>
-    <row r="95" spans="1:33">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A95" s="18" t="s">
         <v>56</v>
       </c>
@@ -4844,7 +4854,7 @@
       <c r="AF95" s="4"/>
       <c r="AG95" s="4"/>
     </row>
-    <row r="96" spans="1:33">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>0</v>
       </c>
@@ -4885,7 +4895,7 @@
       <c r="AF96" s="4"/>
       <c r="AG96" s="4"/>
     </row>
-    <row r="97" spans="1:33">
+    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="B97" s="2" t="s">
         <v>2</v>
@@ -4938,7 +4948,7 @@
       <c r="AF97" s="4"/>
       <c r="AG97" s="4"/>
     </row>
-    <row r="98" spans="1:33">
+    <row r="98" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="B98" s="6">
         <v>3</v>
@@ -4991,7 +5001,7 @@
       <c r="AF98" s="4"/>
       <c r="AG98" s="4"/>
     </row>
-    <row r="99" spans="1:33">
+    <row r="99" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>16</v>
       </c>
@@ -5042,7 +5052,7 @@
       <c r="AF99" s="4"/>
       <c r="AG99" s="4"/>
     </row>
-    <row r="100" spans="1:33">
+    <row r="100" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A100" s="10">
         <v>200</v>
       </c>
@@ -5083,7 +5093,7 @@
       <c r="AF100" s="4"/>
       <c r="AG100" s="4"/>
     </row>
-    <row r="101" spans="1:33">
+    <row r="101" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A101" s="10">
         <v>211</v>
       </c>
@@ -5124,7 +5134,7 @@
       <c r="AF101" s="4"/>
       <c r="AG101" s="4"/>
     </row>
-    <row r="102" spans="1:33">
+    <row r="102" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A102" s="10">
         <v>299</v>
       </c>
@@ -5165,7 +5175,7 @@
       <c r="AF102" s="4"/>
       <c r="AG102" s="4"/>
     </row>
-    <row r="103" spans="1:33">
+    <row r="103" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A103" s="10">
         <v>314</v>
       </c>
@@ -5206,7 +5216,7 @@
       <c r="AF103" s="4"/>
       <c r="AG103" s="4"/>
     </row>
-    <row r="104" spans="1:33">
+    <row r="104" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A104" s="10">
         <v>415</v>
       </c>
@@ -5247,7 +5257,7 @@
       <c r="AF104" s="4"/>
       <c r="AG104" s="4"/>
     </row>
-    <row r="105" spans="1:33">
+    <row r="105" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A105" s="10">
         <v>543</v>
       </c>
@@ -5288,7 +5298,7 @@
       <c r="AF105" s="4"/>
       <c r="AG105" s="4"/>
     </row>
-    <row r="106" spans="1:33">
+    <row r="106" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A106" s="10">
         <v>544</v>
       </c>
@@ -5329,7 +5339,7 @@
       <c r="AF106" s="4"/>
       <c r="AG106" s="4"/>
     </row>
-    <row r="107" spans="1:33">
+    <row r="107" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A107" s="10">
         <v>566</v>
       </c>
@@ -5370,7 +5380,7 @@
       <c r="AF107" s="4"/>
       <c r="AG107" s="4"/>
     </row>
-    <row r="108" spans="1:33">
+    <row r="108" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A108" s="10">
         <v>666</v>
       </c>
@@ -5411,7 +5421,7 @@
       <c r="AF108" s="4"/>
       <c r="AG108" s="4"/>
     </row>
-    <row r="109" spans="1:33">
+    <row r="109" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A109" s="10">
         <v>682</v>
       </c>
@@ -5452,7 +5462,7 @@
       <c r="AF109" s="4"/>
       <c r="AG109" s="4"/>
     </row>
-    <row r="110" spans="1:33">
+    <row r="110" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A110" s="10">
         <v>687</v>
       </c>
@@ -5493,7 +5503,7 @@
       <c r="AF110" s="4"/>
       <c r="AG110" s="4"/>
     </row>
-    <row r="111" spans="1:33">
+    <row r="111" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A111" s="10">
         <v>722</v>
       </c>
@@ -5534,7 +5544,7 @@
       <c r="AF111" s="4"/>
       <c r="AG111" s="4"/>
     </row>
-    <row r="112" spans="1:33">
+    <row r="112" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A112" s="10">
         <v>794</v>
       </c>
@@ -5575,7 +5585,7 @@
       <c r="AF112" s="4"/>
       <c r="AG112" s="4"/>
     </row>
-    <row r="113" spans="1:33">
+    <row r="113" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A113" s="10">
         <v>804</v>
       </c>
@@ -5616,7 +5626,7 @@
       <c r="AF113" s="4"/>
       <c r="AG113" s="4"/>
     </row>
-    <row r="114" spans="1:33">
+    <row r="114" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A114" s="10">
         <v>859</v>
       </c>
@@ -5659,7 +5669,7 @@
       <c r="AF114" s="4"/>
       <c r="AG114" s="4"/>
     </row>
-    <row r="115" spans="1:33">
+    <row r="115" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A115" s="10">
         <v>956</v>
       </c>
@@ -5700,7 +5710,7 @@
       <c r="AF115" s="4"/>
       <c r="AG115" s="4"/>
     </row>
-    <row r="116" spans="1:33">
+    <row r="116" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A116" s="10">
         <v>1039</v>
       </c>
@@ -5741,7 +5751,7 @@
       <c r="AF116" s="4"/>
       <c r="AG116" s="4"/>
     </row>
-    <row r="117" spans="1:33">
+    <row r="117" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A117" s="10">
         <v>1045</v>
       </c>
@@ -5782,7 +5792,7 @@
       <c r="AF117" s="4"/>
       <c r="AG117" s="4"/>
     </row>
-    <row r="118" spans="1:33">
+    <row r="118" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A118" s="10">
         <v>1088</v>
       </c>
@@ -5823,7 +5833,7 @@
       <c r="AF118" s="4"/>
       <c r="AG118" s="4"/>
     </row>
-    <row r="119" spans="1:33">
+    <row r="119" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A119" s="10">
         <v>1150</v>
       </c>
@@ -5864,7 +5874,7 @@
       <c r="AF119" s="4"/>
       <c r="AG119" s="4"/>
     </row>
-    <row r="120" spans="1:33">
+    <row r="120" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A120" s="10">
         <v>1181</v>
       </c>
@@ -5905,7 +5915,7 @@
       <c r="AF120" s="4"/>
       <c r="AG120" s="4"/>
     </row>
-    <row r="121" spans="1:33">
+    <row r="121" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A121" s="10">
         <v>1299</v>
       </c>
@@ -5946,7 +5956,7 @@
       <c r="AF121" s="4"/>
       <c r="AG121" s="4"/>
     </row>
-    <row r="122" spans="1:33">
+    <row r="122" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A122" s="10">
         <v>1388</v>
       </c>
@@ -5987,7 +5997,7 @@
       <c r="AF122" s="4"/>
       <c r="AG122" s="4"/>
     </row>
-    <row r="123" spans="1:33">
+    <row r="123" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A123" s="10">
         <v>1429</v>
       </c>
@@ -6030,7 +6040,7 @@
       <c r="AF123" s="4"/>
       <c r="AG123" s="4"/>
     </row>
-    <row r="124" spans="1:33">
+    <row r="124" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A124" s="10">
         <v>1599</v>
       </c>
@@ -6071,7 +6081,7 @@
       <c r="AF124" s="4"/>
       <c r="AG124" s="4"/>
     </row>
-    <row r="125" spans="1:33">
+    <row r="125" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -6106,7 +6116,7 @@
       <c r="AF125" s="4"/>
       <c r="AG125" s="4"/>
     </row>
-    <row r="126" spans="1:33">
+    <row r="126" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -6141,7 +6151,7 @@
       <c r="AF126" s="4"/>
       <c r="AG126" s="4"/>
     </row>
-    <row r="127" spans="1:33">
+    <row r="127" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -6176,7 +6186,7 @@
       <c r="AF127" s="4"/>
       <c r="AG127" s="4"/>
     </row>
-    <row r="128" spans="1:33">
+    <row r="128" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -6211,7 +6221,7 @@
       <c r="AF128" s="4"/>
       <c r="AG128" s="4"/>
     </row>
-    <row r="129" spans="1:33">
+    <row r="129" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -6246,7 +6256,7 @@
       <c r="AF129" s="4"/>
       <c r="AG129" s="4"/>
     </row>
-    <row r="130" spans="1:33">
+    <row r="130" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -6281,7 +6291,7 @@
       <c r="AF130" s="4"/>
       <c r="AG130" s="4"/>
     </row>
-    <row r="131" spans="1:33">
+    <row r="131" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -6316,7 +6326,7 @@
       <c r="AF131" s="4"/>
       <c r="AG131" s="4"/>
     </row>
-    <row r="132" spans="1:33">
+    <row r="132" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -6351,7 +6361,7 @@
       <c r="AF132" s="4"/>
       <c r="AG132" s="4"/>
     </row>
-    <row r="133" spans="1:33">
+    <row r="133" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -6386,7 +6396,7 @@
       <c r="AF133" s="4"/>
       <c r="AG133" s="4"/>
     </row>
-    <row r="134" spans="1:33">
+    <row r="134" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -6421,7 +6431,7 @@
       <c r="AF134" s="4"/>
       <c r="AG134" s="4"/>
     </row>
-    <row r="135" spans="1:33">
+    <row r="135" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -6456,7 +6466,7 @@
       <c r="AF135" s="4"/>
       <c r="AG135" s="4"/>
     </row>
-    <row r="136" spans="1:33">
+    <row r="136" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
@@ -6491,7 +6501,7 @@
       <c r="AF136" s="4"/>
       <c r="AG136" s="4"/>
     </row>
-    <row r="137" spans="1:33">
+    <row r="137" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
@@ -6526,7 +6536,7 @@
       <c r="AF137" s="4"/>
       <c r="AG137" s="4"/>
     </row>
-    <row r="138" spans="1:33">
+    <row r="138" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A138" s="4"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
@@ -6561,7 +6571,7 @@
       <c r="AF138" s="4"/>
       <c r="AG138" s="4"/>
     </row>
-    <row r="139" spans="1:33">
+    <row r="139" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
@@ -6596,7 +6606,7 @@
       <c r="AF139" s="4"/>
       <c r="AG139" s="4"/>
     </row>
-    <row r="140" spans="1:33">
+    <row r="140" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
@@ -6631,7 +6641,7 @@
       <c r="AF140" s="4"/>
       <c r="AG140" s="4"/>
     </row>
-    <row r="141" spans="1:33">
+    <row r="141" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
@@ -6666,7 +6676,7 @@
       <c r="AF141" s="4"/>
       <c r="AG141" s="4"/>
     </row>
-    <row r="142" spans="1:33">
+    <row r="142" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A142" s="4"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
@@ -6701,7 +6711,7 @@
       <c r="AF142" s="4"/>
       <c r="AG142" s="4"/>
     </row>
-    <row r="143" spans="1:33">
+    <row r="143" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
@@ -6738,7 +6748,7 @@
       <c r="AF143" s="4"/>
       <c r="AG143" s="4"/>
     </row>
-    <row r="144" spans="1:33">
+    <row r="144" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A144" s="18" t="s">
         <v>56</v>
       </c>
@@ -6779,7 +6789,7 @@
       <c r="AF144" s="4"/>
       <c r="AG144" s="4"/>
     </row>
-    <row r="145" spans="1:33">
+    <row r="145" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>0</v>
       </c>
@@ -6820,7 +6830,7 @@
       <c r="AF145" s="4"/>
       <c r="AG145" s="4"/>
     </row>
-    <row r="146" spans="1:33">
+    <row r="146" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
       <c r="B146" s="2" t="s">
         <v>2</v>
@@ -6873,7 +6883,7 @@
       <c r="AF146" s="4"/>
       <c r="AG146" s="4"/>
     </row>
-    <row r="147" spans="1:33">
+    <row r="147" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
       <c r="B147" s="6">
         <v>5</v>
@@ -6926,7 +6936,7 @@
       <c r="AF147" s="4"/>
       <c r="AG147" s="4"/>
     </row>
-    <row r="148" spans="1:33">
+    <row r="148" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>16</v>
       </c>
@@ -6977,7 +6987,7 @@
       <c r="AF148" s="4"/>
       <c r="AG148" s="4"/>
     </row>
-    <row r="149" spans="1:33">
+    <row r="149" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A149" s="10">
         <v>55</v>
       </c>
@@ -7018,7 +7028,7 @@
       <c r="AF149" s="4"/>
       <c r="AG149" s="4"/>
     </row>
-    <row r="150" spans="1:33">
+    <row r="150" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A150" s="10">
         <v>156</v>
       </c>
@@ -7059,7 +7069,7 @@
       <c r="AF150" s="4"/>
       <c r="AG150" s="4"/>
     </row>
-    <row r="151" spans="1:33">
+    <row r="151" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A151" s="10">
         <v>195</v>
       </c>
@@ -7100,7 +7110,7 @@
       <c r="AF151" s="4"/>
       <c r="AG151" s="4"/>
     </row>
-    <row r="152" spans="1:33">
+    <row r="152" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A152" s="10">
         <v>303</v>
       </c>
@@ -7141,7 +7151,7 @@
       <c r="AF152" s="4"/>
       <c r="AG152" s="4"/>
     </row>
-    <row r="153" spans="1:33">
+    <row r="153" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A153" s="10">
         <v>378</v>
       </c>
@@ -7182,7 +7192,7 @@
       <c r="AF153" s="4"/>
       <c r="AG153" s="4"/>
     </row>
-    <row r="154" spans="1:33">
+    <row r="154" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A154" s="10">
         <v>401</v>
       </c>
@@ -7223,7 +7233,7 @@
       <c r="AF154" s="4"/>
       <c r="AG154" s="4"/>
     </row>
-    <row r="155" spans="1:33">
+    <row r="155" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A155" s="10">
         <v>448</v>
       </c>
@@ -7266,7 +7276,7 @@
       <c r="AF155" s="4"/>
       <c r="AG155" s="4"/>
     </row>
-    <row r="156" spans="1:33">
+    <row r="156" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A156" s="10">
         <v>497</v>
       </c>
@@ -7307,7 +7317,7 @@
       <c r="AF156" s="4"/>
       <c r="AG156" s="4"/>
     </row>
-    <row r="157" spans="1:33">
+    <row r="157" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A157" s="10">
         <v>541</v>
       </c>
@@ -7348,7 +7358,7 @@
       <c r="AF157" s="4"/>
       <c r="AG157" s="4"/>
     </row>
-    <row r="158" spans="1:33">
+    <row r="158" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A158" s="10">
         <v>731</v>
       </c>
@@ -7389,7 +7399,7 @@
       <c r="AF158" s="4"/>
       <c r="AG158" s="4"/>
     </row>
-    <row r="159" spans="1:33">
+    <row r="159" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A159" s="10">
         <v>777</v>
       </c>
@@ -7430,7 +7440,7 @@
       <c r="AF159" s="4"/>
       <c r="AG159" s="4"/>
     </row>
-    <row r="160" spans="1:33">
+    <row r="160" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A160" s="10">
         <v>850</v>
       </c>
@@ -7471,7 +7481,7 @@
       <c r="AF160" s="4"/>
       <c r="AG160" s="4"/>
     </row>
-    <row r="161" spans="1:33">
+    <row r="161" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A161" s="10">
         <v>860</v>
       </c>
@@ -7512,7 +7522,7 @@
       <c r="AF161" s="4"/>
       <c r="AG161" s="4"/>
     </row>
-    <row r="162" spans="1:33">
+    <row r="162" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A162" s="10">
         <v>886</v>
       </c>
@@ -7553,7 +7563,7 @@
       <c r="AF162" s="4"/>
       <c r="AG162" s="4"/>
     </row>
-    <row r="163" spans="1:33">
+    <row r="163" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A163" s="10">
         <v>908</v>
       </c>
@@ -7594,7 +7604,7 @@
       <c r="AF163" s="4"/>
       <c r="AG163" s="4"/>
     </row>
-    <row r="164" spans="1:33">
+    <row r="164" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A164" s="10">
         <v>1099</v>
       </c>
@@ -7635,7 +7645,7 @@
       <c r="AF164" s="4"/>
       <c r="AG164" s="4"/>
     </row>
-    <row r="165" spans="1:33">
+    <row r="165" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A165" s="10">
         <v>1217</v>
       </c>
@@ -7676,7 +7686,7 @@
       <c r="AF165" s="4"/>
       <c r="AG165" s="4"/>
     </row>
-    <row r="166" spans="1:33">
+    <row r="166" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A166" s="10">
         <v>1261</v>
       </c>
@@ -7717,7 +7727,7 @@
       <c r="AF166" s="4"/>
       <c r="AG166" s="4"/>
     </row>
-    <row r="167" spans="1:33">
+    <row r="167" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A167" s="10">
         <v>1354</v>
       </c>
@@ -7758,7 +7768,7 @@
       <c r="AF167" s="4"/>
       <c r="AG167" s="4"/>
     </row>
-    <row r="168" spans="1:33">
+    <row r="168" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A168" s="10">
         <v>1373</v>
       </c>
@@ -7799,7 +7809,7 @@
       <c r="AF168" s="4"/>
       <c r="AG168" s="4"/>
     </row>
-    <row r="169" spans="1:33">
+    <row r="169" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A169" s="10">
         <v>1415</v>
       </c>
@@ -7840,7 +7850,7 @@
       <c r="AF169" s="4"/>
       <c r="AG169" s="4"/>
     </row>
-    <row r="170" spans="1:33">
+    <row r="170" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A170" s="10">
         <v>1424</v>
       </c>
@@ -7881,7 +7891,7 @@
       <c r="AF170" s="4"/>
       <c r="AG170" s="4"/>
     </row>
-    <row r="171" spans="1:33">
+    <row r="171" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A171" s="10">
         <v>1438</v>
       </c>
@@ -7922,7 +7932,7 @@
       <c r="AF171" s="4"/>
       <c r="AG171" s="4"/>
     </row>
-    <row r="172" spans="1:33">
+    <row r="172" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A172" s="10">
         <v>1451</v>
       </c>
@@ -7963,7 +7973,7 @@
       <c r="AF172" s="4"/>
       <c r="AG172" s="4"/>
     </row>
-    <row r="173" spans="1:33">
+    <row r="173" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A173" s="10">
         <v>1609</v>
       </c>
@@ -8004,7 +8014,7 @@
       <c r="AF173" s="4"/>
       <c r="AG173" s="4"/>
     </row>
-    <row r="174" spans="1:33">
+    <row r="174" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A174" s="10">
         <v>779</v>
       </c>
@@ -8045,7 +8055,7 @@
       <c r="AF174" s="4"/>
       <c r="AG174" s="4"/>
     </row>
-    <row r="175" spans="1:33">
+    <row r="175" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A175" s="4"/>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
@@ -8080,7 +8090,7 @@
       <c r="AF175" s="4"/>
       <c r="AG175" s="4"/>
     </row>
-    <row r="176" spans="1:33">
+    <row r="176" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
@@ -8115,7 +8125,7 @@
       <c r="AF176" s="4"/>
       <c r="AG176" s="4"/>
     </row>
-    <row r="177" spans="1:33">
+    <row r="177" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A177" s="4"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
@@ -8150,7 +8160,7 @@
       <c r="AF177" s="4"/>
       <c r="AG177" s="4"/>
     </row>
-    <row r="178" spans="1:33">
+    <row r="178" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A178" s="4"/>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
@@ -8185,7 +8195,7 @@
       <c r="AF178" s="4"/>
       <c r="AG178" s="4"/>
     </row>
-    <row r="179" spans="1:33">
+    <row r="179" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A179" s="4"/>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
@@ -8220,7 +8230,7 @@
       <c r="AF179" s="4"/>
       <c r="AG179" s="4"/>
     </row>
-    <row r="180" spans="1:33">
+    <row r="180" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A180" s="4"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
@@ -8255,7 +8265,7 @@
       <c r="AF180" s="4"/>
       <c r="AG180" s="4"/>
     </row>
-    <row r="181" spans="1:33">
+    <row r="181" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A181" s="4"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
@@ -8290,7 +8300,7 @@
       <c r="AF181" s="4"/>
       <c r="AG181" s="4"/>
     </row>
-    <row r="182" spans="1:33">
+    <row r="182" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A182" s="4"/>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
@@ -8325,7 +8335,7 @@
       <c r="AF182" s="4"/>
       <c r="AG182" s="4"/>
     </row>
-    <row r="183" spans="1:33">
+    <row r="183" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A183" s="4"/>
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
@@ -8360,7 +8370,7 @@
       <c r="AF183" s="4"/>
       <c r="AG183" s="4"/>
     </row>
-    <row r="184" spans="1:33">
+    <row r="184" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A184" s="4"/>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
@@ -8395,7 +8405,7 @@
       <c r="AF184" s="4"/>
       <c r="AG184" s="4"/>
     </row>
-    <row r="185" spans="1:33">
+    <row r="185" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A185" s="4"/>
       <c r="B185" s="4"/>
       <c r="C185" s="4"/>
@@ -8430,7 +8440,7 @@
       <c r="AF185" s="4"/>
       <c r="AG185" s="4"/>
     </row>
-    <row r="186" spans="1:33">
+    <row r="186" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A186" s="4"/>
       <c r="B186" s="4"/>
       <c r="C186" s="4"/>
@@ -8465,7 +8475,7 @@
       <c r="AF186" s="4"/>
       <c r="AG186" s="4"/>
     </row>
-    <row r="187" spans="1:33">
+    <row r="187" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A187" s="4"/>
       <c r="B187" s="4"/>
       <c r="C187" s="4"/>
@@ -8500,7 +8510,7 @@
       <c r="AF187" s="4"/>
       <c r="AG187" s="4"/>
     </row>
-    <row r="188" spans="1:33">
+    <row r="188" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A188" s="4"/>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
@@ -8535,7 +8545,7 @@
       <c r="AF188" s="4"/>
       <c r="AG188" s="4"/>
     </row>
-    <row r="189" spans="1:33">
+    <row r="189" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A189" s="4"/>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
@@ -8570,7 +8580,7 @@
       <c r="AF189" s="4"/>
       <c r="AG189" s="4"/>
     </row>
-    <row r="190" spans="1:33">
+    <row r="190" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A190" s="4"/>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
@@ -8605,7 +8615,7 @@
       <c r="AF190" s="4"/>
       <c r="AG190" s="4"/>
     </row>
-    <row r="191" spans="1:33">
+    <row r="191" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A191" s="4"/>
       <c r="B191" s="4"/>
       <c r="C191" s="4"/>
@@ -8640,7 +8650,7 @@
       <c r="AF191" s="4"/>
       <c r="AG191" s="4"/>
     </row>
-    <row r="192" spans="1:33">
+    <row r="192" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A192" s="7"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
@@ -8677,7 +8687,7 @@
       <c r="AF192" s="4"/>
       <c r="AG192" s="4"/>
     </row>
-    <row r="193" spans="1:33">
+    <row r="193" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A193" s="18" t="s">
         <v>56</v>
       </c>
@@ -8718,7 +8728,7 @@
       <c r="AF193" s="4"/>
       <c r="AG193" s="4"/>
     </row>
-    <row r="194" spans="1:33">
+    <row r="194" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>0</v>
       </c>
@@ -8759,7 +8769,7 @@
       <c r="AF194" s="4"/>
       <c r="AG194" s="4"/>
     </row>
-    <row r="195" spans="1:33">
+    <row r="195" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A195" s="5"/>
       <c r="B195" s="2" t="s">
         <v>2</v>
@@ -8812,7 +8822,7 @@
       <c r="AF195" s="4"/>
       <c r="AG195" s="4"/>
     </row>
-    <row r="196" spans="1:33">
+    <row r="196" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A196" s="5"/>
       <c r="B196" s="6">
         <v>6</v>
@@ -8865,7 +8875,7 @@
       <c r="AF196" s="4"/>
       <c r="AG196" s="4"/>
     </row>
-    <row r="197" spans="1:33">
+    <row r="197" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>16</v>
       </c>
@@ -8916,7 +8926,7 @@
       <c r="AF197" s="4"/>
       <c r="AG197" s="4"/>
     </row>
-    <row r="198" spans="1:33">
+    <row r="198" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A198" s="10">
         <v>9</v>
       </c>
@@ -8957,7 +8967,7 @@
       <c r="AF198" s="4"/>
       <c r="AG198" s="4"/>
     </row>
-    <row r="199" spans="1:33">
+    <row r="199" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A199" s="10">
         <v>32</v>
       </c>
@@ -8998,7 +9008,7 @@
       <c r="AF199" s="4"/>
       <c r="AG199" s="4"/>
     </row>
-    <row r="200" spans="1:33">
+    <row r="200" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A200" s="10">
         <v>209</v>
       </c>
@@ -9039,7 +9049,7 @@
       <c r="AF200" s="4"/>
       <c r="AG200" s="4"/>
     </row>
-    <row r="201" spans="1:33">
+    <row r="201" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A201" s="10">
         <v>268</v>
       </c>
@@ -9080,7 +9090,7 @@
       <c r="AF201" s="4"/>
       <c r="AG201" s="4"/>
     </row>
-    <row r="202" spans="1:33">
+    <row r="202" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A202" s="10">
         <v>319</v>
       </c>
@@ -9121,7 +9131,7 @@
       <c r="AF202" s="4"/>
       <c r="AG202" s="4"/>
     </row>
-    <row r="203" spans="1:33">
+    <row r="203" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A203" s="10">
         <v>343</v>
       </c>
@@ -9162,7 +9172,7 @@
       <c r="AF203" s="4"/>
       <c r="AG203" s="4"/>
     </row>
-    <row r="204" spans="1:33">
+    <row r="204" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A204" s="10">
         <v>382</v>
       </c>
@@ -9203,7 +9213,7 @@
       <c r="AF204" s="4"/>
       <c r="AG204" s="4"/>
     </row>
-    <row r="205" spans="1:33">
+    <row r="205" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A205" s="10">
         <v>456</v>
       </c>
@@ -9244,7 +9254,7 @@
       <c r="AF205" s="4"/>
       <c r="AG205" s="4"/>
     </row>
-    <row r="206" spans="1:33">
+    <row r="206" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A206" s="10">
         <v>508</v>
       </c>
@@ -9285,7 +9295,7 @@
       <c r="AF206" s="4"/>
       <c r="AG206" s="4"/>
     </row>
-    <row r="207" spans="1:33">
+    <row r="207" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A207" s="10">
         <v>636</v>
       </c>
@@ -9326,7 +9336,7 @@
       <c r="AF207" s="4"/>
       <c r="AG207" s="4"/>
     </row>
-    <row r="208" spans="1:33">
+    <row r="208" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A208" s="10">
         <v>737</v>
       </c>
@@ -9367,7 +9377,7 @@
       <c r="AF208" s="4"/>
       <c r="AG208" s="4"/>
     </row>
-    <row r="209" spans="1:33">
+    <row r="209" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A209" s="10">
         <v>739</v>
       </c>
@@ -9408,7 +9418,7 @@
       <c r="AF209" s="4"/>
       <c r="AG209" s="4"/>
     </row>
-    <row r="210" spans="1:33">
+    <row r="210" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A210" s="10">
         <v>779</v>
       </c>
@@ -9449,7 +9459,7 @@
       <c r="AF210" s="4"/>
       <c r="AG210" s="4"/>
     </row>
-    <row r="211" spans="1:33">
+    <row r="211" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A211" s="10">
         <v>891</v>
       </c>
@@ -9490,7 +9500,7 @@
       <c r="AF211" s="4"/>
       <c r="AG211" s="4"/>
     </row>
-    <row r="212" spans="1:33">
+    <row r="212" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A212" s="10">
         <v>938</v>
       </c>
@@ -9531,7 +9541,7 @@
       <c r="AF212" s="4"/>
       <c r="AG212" s="4"/>
     </row>
-    <row r="213" spans="1:33">
+    <row r="213" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A213" s="10">
         <v>1042</v>
       </c>
@@ -9572,7 +9582,7 @@
       <c r="AF213" s="4"/>
       <c r="AG213" s="4"/>
     </row>
-    <row r="214" spans="1:33">
+    <row r="214" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A214" s="10">
         <v>1112</v>
       </c>
@@ -9613,7 +9623,7 @@
       <c r="AF214" s="4"/>
       <c r="AG214" s="4"/>
     </row>
-    <row r="215" spans="1:33">
+    <row r="215" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A215" s="10">
         <v>1198</v>
       </c>
@@ -9654,7 +9664,7 @@
       <c r="AF215" s="4"/>
       <c r="AG215" s="4"/>
     </row>
-    <row r="216" spans="1:33">
+    <row r="216" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A216" s="10">
         <v>1284</v>
       </c>
@@ -9695,7 +9705,7 @@
       <c r="AF216" s="4"/>
       <c r="AG216" s="4"/>
     </row>
-    <row r="217" spans="1:33">
+    <row r="217" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A217" s="10">
         <v>1401</v>
       </c>
@@ -9736,7 +9746,7 @@
       <c r="AF217" s="4"/>
       <c r="AG217" s="4"/>
     </row>
-    <row r="218" spans="1:33">
+    <row r="218" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A218" s="10">
         <v>1434</v>
       </c>
@@ -9777,7 +9787,7 @@
       <c r="AF218" s="4"/>
       <c r="AG218" s="4"/>
     </row>
-    <row r="219" spans="1:33">
+    <row r="219" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A219" s="10">
         <v>1520</v>
       </c>
@@ -9818,7 +9828,7 @@
       <c r="AF219" s="4"/>
       <c r="AG219" s="4"/>
     </row>
-    <row r="220" spans="1:33">
+    <row r="220" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A220" s="10">
         <v>1597</v>
       </c>
@@ -9859,7 +9869,7 @@
       <c r="AF220" s="4"/>
       <c r="AG220" s="4"/>
     </row>
-    <row r="221" spans="1:33">
+    <row r="221" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A221" s="10">
         <v>384</v>
       </c>
@@ -9900,7 +9910,7 @@
       <c r="AF221" s="4"/>
       <c r="AG221" s="4"/>
     </row>
-    <row r="222" spans="1:33">
+    <row r="222" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A222" s="4"/>
       <c r="B222" s="4"/>
       <c r="C222" s="4"/>
@@ -9935,7 +9945,7 @@
       <c r="AF222" s="4"/>
       <c r="AG222" s="4"/>
     </row>
-    <row r="223" spans="1:33">
+    <row r="223" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A223" s="4"/>
       <c r="B223" s="4"/>
       <c r="C223" s="4"/>
@@ -9970,7 +9980,7 @@
       <c r="AF223" s="4"/>
       <c r="AG223" s="4"/>
     </row>
-    <row r="224" spans="1:33">
+    <row r="224" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A224" s="4"/>
       <c r="B224" s="4"/>
       <c r="C224" s="4"/>
@@ -10005,7 +10015,7 @@
       <c r="AF224" s="4"/>
       <c r="AG224" s="4"/>
     </row>
-    <row r="225" spans="1:33">
+    <row r="225" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A225" s="4"/>
       <c r="B225" s="4"/>
       <c r="C225" s="4"/>
@@ -10040,7 +10050,7 @@
       <c r="AF225" s="4"/>
       <c r="AG225" s="4"/>
     </row>
-    <row r="226" spans="1:33">
+    <row r="226" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A226" s="4"/>
       <c r="B226" s="4"/>
       <c r="C226" s="4"/>
@@ -10075,7 +10085,7 @@
       <c r="AF226" s="4"/>
       <c r="AG226" s="4"/>
     </row>
-    <row r="227" spans="1:33">
+    <row r="227" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A227" s="4"/>
       <c r="B227" s="4"/>
       <c r="C227" s="4"/>
@@ -10110,7 +10120,7 @@
       <c r="AF227" s="4"/>
       <c r="AG227" s="4"/>
     </row>
-    <row r="228" spans="1:33">
+    <row r="228" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A228" s="4"/>
       <c r="B228" s="4"/>
       <c r="C228" s="4"/>
@@ -10145,7 +10155,7 @@
       <c r="AF228" s="4"/>
       <c r="AG228" s="4"/>
     </row>
-    <row r="229" spans="1:33">
+    <row r="229" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A229" s="4"/>
       <c r="B229" s="4"/>
       <c r="C229" s="4"/>
@@ -10180,7 +10190,7 @@
       <c r="AF229" s="4"/>
       <c r="AG229" s="4"/>
     </row>
-    <row r="230" spans="1:33">
+    <row r="230" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A230" s="4"/>
       <c r="B230" s="4"/>
       <c r="C230" s="4"/>
@@ -10215,7 +10225,7 @@
       <c r="AF230" s="4"/>
       <c r="AG230" s="4"/>
     </row>
-    <row r="231" spans="1:33">
+    <row r="231" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A231" s="4"/>
       <c r="B231" s="4"/>
       <c r="C231" s="4"/>
@@ -10250,7 +10260,7 @@
       <c r="AF231" s="4"/>
       <c r="AG231" s="4"/>
     </row>
-    <row r="232" spans="1:33">
+    <row r="232" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A232" s="4"/>
       <c r="B232" s="4"/>
       <c r="C232" s="4"/>
@@ -10285,7 +10295,7 @@
       <c r="AF232" s="4"/>
       <c r="AG232" s="4"/>
     </row>
-    <row r="233" spans="1:33">
+    <row r="233" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A233" s="4"/>
       <c r="B233" s="4"/>
       <c r="C233" s="4"/>
@@ -10320,7 +10330,7 @@
       <c r="AF233" s="4"/>
       <c r="AG233" s="4"/>
     </row>
-    <row r="234" spans="1:33">
+    <row r="234" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A234" s="4"/>
       <c r="B234" s="4"/>
       <c r="C234" s="4"/>
@@ -10355,7 +10365,7 @@
       <c r="AF234" s="4"/>
       <c r="AG234" s="4"/>
     </row>
-    <row r="235" spans="1:33">
+    <row r="235" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A235" s="4"/>
       <c r="B235" s="4"/>
       <c r="C235" s="4"/>
@@ -10390,7 +10400,7 @@
       <c r="AF235" s="4"/>
       <c r="AG235" s="4"/>
     </row>
-    <row r="236" spans="1:33">
+    <row r="236" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A236" s="4"/>
       <c r="B236" s="4"/>
       <c r="C236" s="4"/>
@@ -10425,7 +10435,7 @@
       <c r="AF236" s="4"/>
       <c r="AG236" s="4"/>
     </row>
-    <row r="237" spans="1:33">
+    <row r="237" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A237" s="4"/>
       <c r="B237" s="4"/>
       <c r="C237" s="4"/>
@@ -10460,7 +10470,7 @@
       <c r="AF237" s="4"/>
       <c r="AG237" s="4"/>
     </row>
-    <row r="238" spans="1:33">
+    <row r="238" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A238" s="4"/>
       <c r="B238" s="4"/>
       <c r="C238" s="4"/>
@@ -10495,7 +10505,7 @@
       <c r="AF238" s="4"/>
       <c r="AG238" s="4"/>
     </row>
-    <row r="239" spans="1:33">
+    <row r="239" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A239" s="4"/>
       <c r="B239" s="4"/>
       <c r="C239" s="4"/>
@@ -10530,7 +10540,7 @@
       <c r="AF239" s="4"/>
       <c r="AG239" s="4"/>
     </row>
-    <row r="240" spans="1:33">
+    <row r="240" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A240" s="4"/>
       <c r="B240" s="4"/>
       <c r="C240" s="4"/>
@@ -10565,7 +10575,7 @@
       <c r="AF240" s="4"/>
       <c r="AG240" s="4"/>
     </row>
-    <row r="241" spans="1:33">
+    <row r="241" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A241" s="7"/>
       <c r="B241" s="7"/>
       <c r="C241" s="7"/>
@@ -10602,7 +10612,7 @@
       <c r="AF241" s="4"/>
       <c r="AG241" s="4"/>
     </row>
-    <row r="242" spans="1:33">
+    <row r="242" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A242" s="18" t="s">
         <v>56</v>
       </c>
@@ -10643,7 +10653,7 @@
       <c r="AF242" s="4"/>
       <c r="AG242" s="4"/>
     </row>
-    <row r="243" spans="1:33">
+    <row r="243" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>0</v>
       </c>
@@ -10684,7 +10694,7 @@
       <c r="AF243" s="4"/>
       <c r="AG243" s="4"/>
     </row>
-    <row r="244" spans="1:33">
+    <row r="244" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A244" s="5"/>
       <c r="B244" s="2" t="s">
         <v>2</v>
@@ -10737,7 +10747,7 @@
       <c r="AF244" s="4"/>
       <c r="AG244" s="4"/>
     </row>
-    <row r="245" spans="1:33">
+    <row r="245" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A245" s="5"/>
       <c r="B245" s="6">
         <v>8</v>
@@ -10790,7 +10800,7 @@
       <c r="AF245" s="4"/>
       <c r="AG245" s="4"/>
     </row>
-    <row r="246" spans="1:33">
+    <row r="246" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>16</v>
       </c>
@@ -10841,7 +10851,7 @@
       <c r="AF246" s="4"/>
       <c r="AG246" s="4"/>
     </row>
-    <row r="247" spans="1:33">
+    <row r="247" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A247" s="10">
         <v>55</v>
       </c>
@@ -10882,7 +10892,7 @@
       <c r="AF247" s="4"/>
       <c r="AG247" s="4"/>
     </row>
-    <row r="248" spans="1:33">
+    <row r="248" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A248" s="10">
         <v>156</v>
       </c>
@@ -10923,7 +10933,7 @@
       <c r="AF248" s="4"/>
       <c r="AG248" s="4"/>
     </row>
-    <row r="249" spans="1:33">
+    <row r="249" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A249" s="10">
         <v>195</v>
       </c>
@@ -10964,7 +10974,7 @@
       <c r="AF249" s="4"/>
       <c r="AG249" s="4"/>
     </row>
-    <row r="250" spans="1:33">
+    <row r="250" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A250" s="10">
         <v>303</v>
       </c>
@@ -11005,7 +11015,7 @@
       <c r="AF250" s="4"/>
       <c r="AG250" s="4"/>
     </row>
-    <row r="251" spans="1:33">
+    <row r="251" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A251" s="10">
         <v>378</v>
       </c>
@@ -11046,7 +11056,7 @@
       <c r="AF251" s="4"/>
       <c r="AG251" s="4"/>
     </row>
-    <row r="252" spans="1:33">
+    <row r="252" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A252" s="10">
         <v>401</v>
       </c>
@@ -11087,7 +11097,7 @@
       <c r="AF252" s="4"/>
       <c r="AG252" s="4"/>
     </row>
-    <row r="253" spans="1:33">
+    <row r="253" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A253" s="10">
         <v>448</v>
       </c>
@@ -11130,7 +11140,7 @@
       <c r="AF253" s="4"/>
       <c r="AG253" s="4"/>
     </row>
-    <row r="254" spans="1:33">
+    <row r="254" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A254" s="10">
         <v>497</v>
       </c>
@@ -11171,7 +11181,7 @@
       <c r="AF254" s="4"/>
       <c r="AG254" s="4"/>
     </row>
-    <row r="255" spans="1:33">
+    <row r="255" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A255" s="10">
         <v>541</v>
       </c>
@@ -11212,7 +11222,7 @@
       <c r="AF255" s="4"/>
       <c r="AG255" s="4"/>
     </row>
-    <row r="256" spans="1:33">
+    <row r="256" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A256" s="10">
         <v>731</v>
       </c>
@@ -11253,7 +11263,7 @@
       <c r="AF256" s="4"/>
       <c r="AG256" s="4"/>
     </row>
-    <row r="257" spans="1:33">
+    <row r="257" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A257" s="10">
         <v>777</v>
       </c>
@@ -11294,7 +11304,7 @@
       <c r="AF257" s="4"/>
       <c r="AG257" s="4"/>
     </row>
-    <row r="258" spans="1:33">
+    <row r="258" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A258" s="10">
         <v>779</v>
       </c>
@@ -11335,7 +11345,7 @@
       <c r="AF258" s="4"/>
       <c r="AG258" s="4"/>
     </row>
-    <row r="259" spans="1:33">
+    <row r="259" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A259" s="10">
         <v>850</v>
       </c>
@@ -11376,7 +11386,7 @@
       <c r="AF259" s="4"/>
       <c r="AG259" s="4"/>
     </row>
-    <row r="260" spans="1:33">
+    <row r="260" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A260" s="10">
         <v>860</v>
       </c>
@@ -11417,7 +11427,7 @@
       <c r="AF260" s="4"/>
       <c r="AG260" s="4"/>
     </row>
-    <row r="261" spans="1:33">
+    <row r="261" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A261" s="10">
         <v>886</v>
       </c>
@@ -11458,7 +11468,7 @@
       <c r="AF261" s="4"/>
       <c r="AG261" s="4"/>
     </row>
-    <row r="262" spans="1:33">
+    <row r="262" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A262" s="10">
         <v>908</v>
       </c>
@@ -11499,7 +11509,7 @@
       <c r="AF262" s="4"/>
       <c r="AG262" s="4"/>
     </row>
-    <row r="263" spans="1:33">
+    <row r="263" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A263" s="10">
         <v>1099</v>
       </c>
@@ -11540,7 +11550,7 @@
       <c r="AF263" s="4"/>
       <c r="AG263" s="4"/>
     </row>
-    <row r="264" spans="1:33">
+    <row r="264" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A264" s="10">
         <v>1217</v>
       </c>
@@ -11581,7 +11591,7 @@
       <c r="AF264" s="4"/>
       <c r="AG264" s="4"/>
     </row>
-    <row r="265" spans="1:33">
+    <row r="265" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A265" s="10">
         <v>1261</v>
       </c>
@@ -11622,7 +11632,7 @@
       <c r="AF265" s="4"/>
       <c r="AG265" s="4"/>
     </row>
-    <row r="266" spans="1:33">
+    <row r="266" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A266" s="10">
         <v>1354</v>
       </c>
@@ -11663,7 +11673,7 @@
       <c r="AF266" s="4"/>
       <c r="AG266" s="4"/>
     </row>
-    <row r="267" spans="1:33">
+    <row r="267" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A267" s="10">
         <v>1373</v>
       </c>
@@ -11704,7 +11714,7 @@
       <c r="AF267" s="4"/>
       <c r="AG267" s="4"/>
     </row>
-    <row r="268" spans="1:33">
+    <row r="268" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A268" s="10">
         <v>1415</v>
       </c>
@@ -11745,7 +11755,7 @@
       <c r="AF268" s="4"/>
       <c r="AG268" s="4"/>
     </row>
-    <row r="269" spans="1:33">
+    <row r="269" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A269" s="10">
         <v>1424</v>
       </c>
@@ -11786,7 +11796,7 @@
       <c r="AF269" s="4"/>
       <c r="AG269" s="4"/>
     </row>
-    <row r="270" spans="1:33">
+    <row r="270" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A270" s="10">
         <v>1438</v>
       </c>
@@ -11827,7 +11837,7 @@
       <c r="AF270" s="4"/>
       <c r="AG270" s="4"/>
     </row>
-    <row r="271" spans="1:33">
+    <row r="271" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A271" s="10">
         <v>1451</v>
       </c>
@@ -11868,7 +11878,7 @@
       <c r="AF271" s="4"/>
       <c r="AG271" s="4"/>
     </row>
-    <row r="272" spans="1:33">
+    <row r="272" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A272" s="10">
         <v>1609</v>
       </c>
@@ -11909,7 +11919,7 @@
       <c r="AF272" s="4"/>
       <c r="AG272" s="4"/>
     </row>
-    <row r="273" spans="1:33">
+    <row r="273" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A273" s="4"/>
       <c r="B273" s="4"/>
       <c r="C273" s="4"/>
@@ -11944,7 +11954,7 @@
       <c r="AF273" s="4"/>
       <c r="AG273" s="4"/>
     </row>
-    <row r="274" spans="1:33">
+    <row r="274" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A274" s="4"/>
       <c r="B274" s="4"/>
       <c r="C274" s="4"/>
@@ -11979,7 +11989,7 @@
       <c r="AF274" s="4"/>
       <c r="AG274" s="4"/>
     </row>
-    <row r="275" spans="1:33">
+    <row r="275" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A275" s="4"/>
       <c r="B275" s="4"/>
       <c r="C275" s="4"/>
@@ -12014,7 +12024,7 @@
       <c r="AF275" s="4"/>
       <c r="AG275" s="4"/>
     </row>
-    <row r="276" spans="1:33">
+    <row r="276" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A276" s="4"/>
       <c r="B276" s="4"/>
       <c r="C276" s="4"/>
@@ -12049,7 +12059,7 @@
       <c r="AF276" s="4"/>
       <c r="AG276" s="4"/>
     </row>
-    <row r="277" spans="1:33">
+    <row r="277" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A277" s="4"/>
       <c r="B277" s="4"/>
       <c r="C277" s="4"/>
@@ -12084,7 +12094,7 @@
       <c r="AF277" s="4"/>
       <c r="AG277" s="4"/>
     </row>
-    <row r="278" spans="1:33">
+    <row r="278" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A278" s="4"/>
       <c r="B278" s="4"/>
       <c r="C278" s="4"/>
@@ -12119,7 +12129,7 @@
       <c r="AF278" s="4"/>
       <c r="AG278" s="4"/>
     </row>
-    <row r="279" spans="1:33">
+    <row r="279" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A279" s="4"/>
       <c r="B279" s="4"/>
       <c r="C279" s="4"/>
@@ -12154,7 +12164,7 @@
       <c r="AF279" s="4"/>
       <c r="AG279" s="4"/>
     </row>
-    <row r="280" spans="1:33">
+    <row r="280" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A280" s="4"/>
       <c r="B280" s="4"/>
       <c r="C280" s="4"/>
@@ -12189,7 +12199,7 @@
       <c r="AF280" s="4"/>
       <c r="AG280" s="4"/>
     </row>
-    <row r="281" spans="1:33">
+    <row r="281" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A281" s="4"/>
       <c r="B281" s="4"/>
       <c r="C281" s="4"/>
@@ -12224,7 +12234,7 @@
       <c r="AF281" s="4"/>
       <c r="AG281" s="4"/>
     </row>
-    <row r="282" spans="1:33">
+    <row r="282" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A282" s="4"/>
       <c r="B282" s="4"/>
       <c r="C282" s="4"/>
@@ -12259,7 +12269,7 @@
       <c r="AF282" s="4"/>
       <c r="AG282" s="4"/>
     </row>
-    <row r="283" spans="1:33">
+    <row r="283" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A283" s="4"/>
       <c r="B283" s="4"/>
       <c r="C283" s="4"/>
@@ -12294,7 +12304,7 @@
       <c r="AF283" s="4"/>
       <c r="AG283" s="4"/>
     </row>
-    <row r="284" spans="1:33">
+    <row r="284" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A284" s="4"/>
       <c r="B284" s="4"/>
       <c r="C284" s="4"/>
@@ -12329,7 +12339,7 @@
       <c r="AF284" s="4"/>
       <c r="AG284" s="4"/>
     </row>
-    <row r="285" spans="1:33">
+    <row r="285" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A285" s="4"/>
       <c r="B285" s="4"/>
       <c r="C285" s="4"/>
@@ -12364,7 +12374,7 @@
       <c r="AF285" s="4"/>
       <c r="AG285" s="4"/>
     </row>
-    <row r="286" spans="1:33">
+    <row r="286" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A286" s="4"/>
       <c r="B286" s="4"/>
       <c r="C286" s="4"/>
@@ -12399,7 +12409,7 @@
       <c r="AF286" s="4"/>
       <c r="AG286" s="4"/>
     </row>
-    <row r="287" spans="1:33">
+    <row r="287" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A287" s="4"/>
       <c r="B287" s="4"/>
       <c r="C287" s="4"/>
@@ -12434,7 +12444,7 @@
       <c r="AF287" s="4"/>
       <c r="AG287" s="4"/>
     </row>
-    <row r="288" spans="1:33">
+    <row r="288" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A288" s="4"/>
       <c r="B288" s="4"/>
       <c r="C288" s="4"/>
@@ -12469,7 +12479,7 @@
       <c r="AF288" s="4"/>
       <c r="AG288" s="4"/>
     </row>
-    <row r="289" spans="1:33">
+    <row r="289" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A289" s="4"/>
       <c r="B289" s="4"/>
       <c r="C289" s="4"/>
@@ -12504,7 +12514,7 @@
       <c r="AF289" s="4"/>
       <c r="AG289" s="4"/>
     </row>
-    <row r="290" spans="1:33">
+    <row r="290" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A290" s="7"/>
       <c r="B290" s="7"/>
       <c r="C290" s="7"/>
@@ -12541,7 +12551,7 @@
       <c r="AF290" s="4"/>
       <c r="AG290" s="4"/>
     </row>
-    <row r="291" spans="1:33">
+    <row r="291" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A291" s="18" t="s">
         <v>56</v>
       </c>
@@ -12582,7 +12592,7 @@
       <c r="AF291" s="4"/>
       <c r="AG291" s="4"/>
     </row>
-    <row r="292" spans="1:33">
+    <row r="292" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>0</v>
       </c>
@@ -12623,7 +12633,7 @@
       <c r="AF292" s="4"/>
       <c r="AG292" s="4"/>
     </row>
-    <row r="293" spans="1:33">
+    <row r="293" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A293" s="5"/>
       <c r="B293" s="2" t="s">
         <v>2</v>
@@ -12676,7 +12686,7 @@
       <c r="AF293" s="4"/>
       <c r="AG293" s="4"/>
     </row>
-    <row r="294" spans="1:33">
+    <row r="294" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A294" s="5"/>
       <c r="B294" s="6">
         <v>9</v>
@@ -12729,7 +12739,7 @@
       <c r="AF294" s="4"/>
       <c r="AG294" s="4"/>
     </row>
-    <row r="295" spans="1:33">
+    <row r="295" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>16</v>
       </c>
@@ -12780,7 +12790,7 @@
       <c r="AF295" s="4"/>
       <c r="AG295" s="4"/>
     </row>
-    <row r="296" spans="1:33">
+    <row r="296" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A296" s="10">
         <v>9</v>
       </c>
@@ -12821,7 +12831,7 @@
       <c r="AF296" s="4"/>
       <c r="AG296" s="4"/>
     </row>
-    <row r="297" spans="1:33">
+    <row r="297" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A297" s="10">
         <v>32</v>
       </c>
@@ -12862,7 +12872,7 @@
       <c r="AF297" s="4"/>
       <c r="AG297" s="4"/>
     </row>
-    <row r="298" spans="1:33">
+    <row r="298" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A298" s="10">
         <v>209</v>
       </c>
@@ -12903,7 +12913,7 @@
       <c r="AF298" s="4"/>
       <c r="AG298" s="4"/>
     </row>
-    <row r="299" spans="1:33">
+    <row r="299" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A299" s="10">
         <v>268</v>
       </c>
@@ -12944,7 +12954,7 @@
       <c r="AF299" s="4"/>
       <c r="AG299" s="4"/>
     </row>
-    <row r="300" spans="1:33">
+    <row r="300" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A300" s="10">
         <v>319</v>
       </c>
@@ -12985,7 +12995,7 @@
       <c r="AF300" s="4"/>
       <c r="AG300" s="4"/>
     </row>
-    <row r="301" spans="1:33">
+    <row r="301" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A301" s="10">
         <v>343</v>
       </c>
@@ -13028,7 +13038,7 @@
       <c r="AF301" s="4"/>
       <c r="AG301" s="4"/>
     </row>
-    <row r="302" spans="1:33">
+    <row r="302" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A302" s="10">
         <v>382</v>
       </c>
@@ -13069,7 +13079,7 @@
       <c r="AF302" s="4"/>
       <c r="AG302" s="4"/>
     </row>
-    <row r="303" spans="1:33">
+    <row r="303" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A303" s="10">
         <v>384</v>
       </c>
@@ -13110,7 +13120,7 @@
       <c r="AF303" s="4"/>
       <c r="AG303" s="4"/>
     </row>
-    <row r="304" spans="1:33">
+    <row r="304" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A304" s="10">
         <v>456</v>
       </c>
@@ -13151,7 +13161,7 @@
       <c r="AF304" s="4"/>
       <c r="AG304" s="4"/>
     </row>
-    <row r="305" spans="1:33">
+    <row r="305" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A305" s="10">
         <v>508</v>
       </c>
@@ -13194,7 +13204,7 @@
       <c r="AF305" s="4"/>
       <c r="AG305" s="4"/>
     </row>
-    <row r="306" spans="1:33">
+    <row r="306" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A306" s="10">
         <v>636</v>
       </c>
@@ -13235,7 +13245,7 @@
       <c r="AF306" s="4"/>
       <c r="AG306" s="4"/>
     </row>
-    <row r="307" spans="1:33">
+    <row r="307" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A307" s="10">
         <v>737</v>
       </c>
@@ -13276,7 +13286,7 @@
       <c r="AF307" s="4"/>
       <c r="AG307" s="4"/>
     </row>
-    <row r="308" spans="1:33">
+    <row r="308" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A308" s="10">
         <v>739</v>
       </c>
@@ -13317,7 +13327,7 @@
       <c r="AF308" s="4"/>
       <c r="AG308" s="4"/>
     </row>
-    <row r="309" spans="1:33">
+    <row r="309" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A309" s="10">
         <v>779</v>
       </c>
@@ -13358,7 +13368,7 @@
       <c r="AF309" s="4"/>
       <c r="AG309" s="4"/>
     </row>
-    <row r="310" spans="1:33">
+    <row r="310" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A310" s="10">
         <v>891</v>
       </c>
@@ -13399,7 +13409,7 @@
       <c r="AF310" s="4"/>
       <c r="AG310" s="4"/>
     </row>
-    <row r="311" spans="1:33">
+    <row r="311" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A311" s="10">
         <v>938</v>
       </c>
@@ -13440,7 +13450,7 @@
       <c r="AF311" s="4"/>
       <c r="AG311" s="4"/>
     </row>
-    <row r="312" spans="1:33">
+    <row r="312" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A312" s="10">
         <v>1042</v>
       </c>
@@ -13481,7 +13491,7 @@
       <c r="AF312" s="4"/>
       <c r="AG312" s="4"/>
     </row>
-    <row r="313" spans="1:33">
+    <row r="313" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A313" s="10">
         <v>1112</v>
       </c>
@@ -13522,7 +13532,7 @@
       <c r="AF313" s="4"/>
       <c r="AG313" s="4"/>
     </row>
-    <row r="314" spans="1:33">
+    <row r="314" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A314" s="10">
         <v>1198</v>
       </c>
@@ -13565,7 +13575,7 @@
       <c r="AF314" s="4"/>
       <c r="AG314" s="4"/>
     </row>
-    <row r="315" spans="1:33">
+    <row r="315" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A315" s="10">
         <v>1284</v>
       </c>
@@ -13606,7 +13616,7 @@
       <c r="AF315" s="4"/>
       <c r="AG315" s="4"/>
     </row>
-    <row r="316" spans="1:33">
+    <row r="316" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A316" s="10">
         <v>1401</v>
       </c>
@@ -13647,7 +13657,7 @@
       <c r="AF316" s="4"/>
       <c r="AG316" s="4"/>
     </row>
-    <row r="317" spans="1:33">
+    <row r="317" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A317" s="10">
         <v>1434</v>
       </c>
@@ -13688,7 +13698,7 @@
       <c r="AF317" s="4"/>
       <c r="AG317" s="4"/>
     </row>
-    <row r="318" spans="1:33">
+    <row r="318" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A318" s="10">
         <v>1520</v>
       </c>
@@ -13729,7 +13739,7 @@
       <c r="AF318" s="4"/>
       <c r="AG318" s="4"/>
     </row>
-    <row r="319" spans="1:33">
+    <row r="319" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A319" s="10">
         <v>1597</v>
       </c>
@@ -13770,7 +13780,7 @@
       <c r="AF319" s="4"/>
       <c r="AG319" s="4"/>
     </row>
-    <row r="320" spans="1:33">
+    <row r="320" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A320" s="4"/>
       <c r="B320" s="4"/>
       <c r="C320" s="4"/>
@@ -13805,7 +13815,7 @@
       <c r="AF320" s="4"/>
       <c r="AG320" s="4"/>
     </row>
-    <row r="321" spans="1:33">
+    <row r="321" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A321" s="4"/>
       <c r="B321" s="4"/>
       <c r="C321" s="4"/>
@@ -13840,7 +13850,7 @@
       <c r="AF321" s="4"/>
       <c r="AG321" s="4"/>
     </row>
-    <row r="322" spans="1:33">
+    <row r="322" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A322" s="4"/>
       <c r="B322" s="4"/>
       <c r="C322" s="4"/>
@@ -13875,7 +13885,7 @@
       <c r="AF322" s="4"/>
       <c r="AG322" s="4"/>
     </row>
-    <row r="323" spans="1:33">
+    <row r="323" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A323" s="4"/>
       <c r="B323" s="4"/>
       <c r="C323" s="4"/>
@@ -13910,7 +13920,7 @@
       <c r="AF323" s="4"/>
       <c r="AG323" s="4"/>
     </row>
-    <row r="324" spans="1:33">
+    <row r="324" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A324" s="4"/>
       <c r="B324" s="4"/>
       <c r="C324" s="4"/>
@@ -13945,7 +13955,7 @@
       <c r="AF324" s="4"/>
       <c r="AG324" s="4"/>
     </row>
-    <row r="325" spans="1:33">
+    <row r="325" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A325" s="4"/>
       <c r="B325" s="4"/>
       <c r="C325" s="4"/>
@@ -13980,7 +13990,7 @@
       <c r="AF325" s="4"/>
       <c r="AG325" s="4"/>
     </row>
-    <row r="326" spans="1:33">
+    <row r="326" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A326" s="4"/>
       <c r="B326" s="4"/>
       <c r="C326" s="4"/>
@@ -14015,7 +14025,7 @@
       <c r="AF326" s="4"/>
       <c r="AG326" s="4"/>
     </row>
-    <row r="327" spans="1:33">
+    <row r="327" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A327" s="4"/>
       <c r="B327" s="4"/>
       <c r="C327" s="4"/>
@@ -14050,7 +14060,7 @@
       <c r="AF327" s="4"/>
       <c r="AG327" s="4"/>
     </row>
-    <row r="328" spans="1:33">
+    <row r="328" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A328" s="4"/>
       <c r="B328" s="4"/>
       <c r="C328" s="4"/>
@@ -14085,7 +14095,7 @@
       <c r="AF328" s="4"/>
       <c r="AG328" s="4"/>
     </row>
-    <row r="329" spans="1:33">
+    <row r="329" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A329" s="4"/>
       <c r="B329" s="4"/>
       <c r="C329" s="4"/>
@@ -14120,7 +14130,7 @@
       <c r="AF329" s="4"/>
       <c r="AG329" s="4"/>
     </row>
-    <row r="330" spans="1:33">
+    <row r="330" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A330" s="4"/>
       <c r="B330" s="4"/>
       <c r="C330" s="4"/>
@@ -14155,7 +14165,7 @@
       <c r="AF330" s="4"/>
       <c r="AG330" s="4"/>
     </row>
-    <row r="331" spans="1:33">
+    <row r="331" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A331" s="4"/>
       <c r="B331" s="4"/>
       <c r="C331" s="4"/>
@@ -14190,7 +14200,7 @@
       <c r="AF331" s="4"/>
       <c r="AG331" s="4"/>
     </row>
-    <row r="332" spans="1:33">
+    <row r="332" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A332" s="4"/>
       <c r="B332" s="4"/>
       <c r="C332" s="4"/>
@@ -14225,7 +14235,7 @@
       <c r="AF332" s="4"/>
       <c r="AG332" s="4"/>
     </row>
-    <row r="333" spans="1:33">
+    <row r="333" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A333" s="4"/>
       <c r="B333" s="4"/>
       <c r="C333" s="4"/>
@@ -14260,7 +14270,7 @@
       <c r="AF333" s="4"/>
       <c r="AG333" s="4"/>
     </row>
-    <row r="334" spans="1:33">
+    <row r="334" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A334" s="4"/>
       <c r="B334" s="4"/>
       <c r="C334" s="4"/>
@@ -14295,7 +14305,7 @@
       <c r="AF334" s="4"/>
       <c r="AG334" s="4"/>
     </row>
-    <row r="335" spans="1:33">
+    <row r="335" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A335" s="4"/>
       <c r="B335" s="4"/>
       <c r="C335" s="4"/>
@@ -14330,7 +14340,7 @@
       <c r="AF335" s="4"/>
       <c r="AG335" s="4"/>
     </row>
-    <row r="336" spans="1:33">
+    <row r="336" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A336" s="4"/>
       <c r="B336" s="4"/>
       <c r="C336" s="4"/>
@@ -14365,7 +14375,7 @@
       <c r="AF336" s="4"/>
       <c r="AG336" s="4"/>
     </row>
-    <row r="337" spans="1:33">
+    <row r="337" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A337" s="4"/>
       <c r="B337" s="4"/>
       <c r="C337" s="4"/>
@@ -14400,7 +14410,7 @@
       <c r="AF337" s="4"/>
       <c r="AG337" s="4"/>
     </row>
-    <row r="338" spans="1:33">
+    <row r="338" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A338" s="4"/>
       <c r="B338" s="4"/>
       <c r="C338" s="4"/>
@@ -14435,7 +14445,7 @@
       <c r="AF338" s="4"/>
       <c r="AG338" s="4"/>
     </row>
-    <row r="339" spans="1:33">
+    <row r="339" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A339" s="7"/>
       <c r="B339" s="7"/>
       <c r="C339" s="7"/>
@@ -14472,7 +14482,7 @@
       <c r="AF339" s="4"/>
       <c r="AG339" s="4"/>
     </row>
-    <row r="340" spans="1:33">
+    <row r="340" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A340" s="18" t="s">
         <v>56</v>
       </c>
@@ -14513,7 +14523,7 @@
       <c r="AF340" s="4"/>
       <c r="AG340" s="4"/>
     </row>
-    <row r="341" spans="1:33">
+    <row r="341" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A341" s="4"/>
       <c r="B341" s="4"/>
       <c r="C341" s="4"/>
@@ -14548,7 +14558,7 @@
       <c r="AF341" s="4"/>
       <c r="AG341" s="4"/>
     </row>
-    <row r="342" spans="1:33">
+    <row r="342" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A342" s="4"/>
       <c r="B342" s="4"/>
       <c r="C342" s="4"/>
@@ -14583,7 +14593,7 @@
       <c r="AF342" s="4"/>
       <c r="AG342" s="4"/>
     </row>
-    <row r="343" spans="1:33">
+    <row r="343" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A343" s="4"/>
       <c r="B343" s="4"/>
       <c r="C343" s="4"/>
@@ -14618,7 +14628,7 @@
       <c r="AF343" s="4"/>
       <c r="AG343" s="4"/>
     </row>
-    <row r="344" spans="1:33">
+    <row r="344" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A344" s="4"/>
       <c r="B344" s="4"/>
       <c r="C344" s="4"/>

</xml_diff>